<commit_message>
Cleaned up the Excel comparison
</commit_message>
<xml_diff>
--- a/assets/img/posts/2023-11-13-full-apple-watch-comparison/AppleWatchComparison.xlsx
+++ b/assets/img/posts/2023-11-13-full-apple-watch-comparison/AppleWatchComparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattpopovich/Documents/git/mattpopovich.com/assets/img/posts/2023-11-13-full-apple-watch-comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5772C009-BAEC-FC46-9EF1-E9CB19CF2D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A531CBF-FEE4-3D43-921B-A81663182F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9520" yWindow="5160" windowWidth="32160" windowHeight="22400" xr2:uid="{7EE77E98-B3CA-5848-BC57-E527922C940D}"/>
+    <workbookView xWindow="2400" yWindow="2240" windowWidth="35920" windowHeight="24360" xr2:uid="{7EE77E98-B3CA-5848-BC57-E527922C940D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="84">
   <si>
     <t>Ultra 2</t>
   </si>
@@ -146,12 +146,6 @@
     <t>Emergency SOS</t>
   </si>
   <si>
-    <t>Wi-Fi and Bluetooth 4.2</t>
-  </si>
-  <si>
-    <t>GPS/GNSS and barometric altimeter</t>
-  </si>
-  <si>
     <t>Retina LTPO OLED display, up to 1000 nits</t>
   </si>
   <si>
@@ -161,36 +155,18 @@
     <t>S4 SiP with 64-bit dual-core processor; W3 wireless chip</t>
   </si>
   <si>
-    <t>Digital Crown with haptic feedback</t>
-  </si>
-  <si>
     <t>Electrical heart sensor and second-generation optical heart sensor</t>
   </si>
   <si>
-    <t>Emergency SOS9 and Fall Detection</t>
-  </si>
-  <si>
     <t>16GB capacity</t>
   </si>
   <si>
     <t>Always-On Retina LTPO OLED display, up to 1000 nits</t>
   </si>
   <si>
-    <t>Ion-X glass display on aluminum cases; sapphire crystal display on stainless steel, titanium, and ceramic cases</t>
-  </si>
-  <si>
     <t>Ion-X glass display on aluminum cases; sapphire crystal display on stainless steel cases</t>
   </si>
   <si>
-    <t>S5 SiP with 64-bit dual-core processor; W3 wireless chip</t>
-  </si>
-  <si>
-    <t>International emergency calling,10 Emergency SOS,9 and Fall Detection</t>
-  </si>
-  <si>
-    <t>LTE and UMTS, Wi-Fi, and Bluetooth 5.0</t>
-  </si>
-  <si>
     <t>GPS/GNSS, compass, and barometric altimeter</t>
   </si>
   <si>
@@ -200,63 +176,21 @@
     <t>Second-generation optical heart sensor</t>
   </si>
   <si>
-    <t>High and low heart rate notifications, irregular rhythm notification, and ECG app; sleep stages</t>
-  </si>
-  <si>
     <t>High and low heart rate notifications, irregular rhythm notification; sleep stages</t>
   </si>
   <si>
-    <t>GPS/GNSS, compass, and always-on altimeter</t>
-  </si>
-  <si>
     <t>Ion-X glass display on aluminum cases; sapphire crystal display on stainless steel and titanium cases</t>
   </si>
   <si>
-    <t>S6 SiP with 64-bit dual-core processor; W3 wireless chip; U1 chip (Ultra Wideband)27</t>
-  </si>
-  <si>
-    <t>Blood oxygen sensor;4 electrical heart sensor and third-generation optical heart sensor</t>
-  </si>
-  <si>
-    <t>S8 SiP with 64-bit dual-core processor; W3 wireless chip</t>
-  </si>
-  <si>
-    <t>Digital Crown with haptic feedback; Siri</t>
-  </si>
-  <si>
-    <t>International emergency calling,10 Emergency SOS,9 Crash Detection,9 and Fall Detection</t>
-  </si>
-  <si>
-    <t>LTE and UMTS,Wi-Fi 4 (802.11n), and Bluetooth 5.3</t>
-  </si>
-  <si>
-    <t>S7 SiP with 64-bit dual-core processor; W3 wireless chip; U1 chip (Ultra Wideband)27</t>
-  </si>
-  <si>
     <t>Fast charge time</t>
   </si>
   <si>
     <t>*no fast charge time*</t>
   </si>
   <si>
-    <t>S8 SiP with 64-bit dual-core processor; W3 wireless chip; U1 chip (Ultra Wideband)27</t>
-  </si>
-  <si>
-    <t>Temperature sensor,7 blood oxygen sensor;4 electrical heart sensor and third-generation optical heart sensor</t>
-  </si>
-  <si>
     <t>Dust resistant (IP6X)</t>
   </si>
   <si>
-    <t>Always-On Retina LTPO OLED display, up to 2000 nits</t>
-  </si>
-  <si>
-    <t>S9 SiP with 64-bit dual-core processor; W3 wireless chip; second-generation Ultra Wideband chip27</t>
-  </si>
-  <si>
-    <t>Digital Crown with haptic feedback; side button; double tap gesture; on-device Siri</t>
-  </si>
-  <si>
     <t>64GB capacity</t>
   </si>
   <si>
@@ -266,18 +200,6 @@
     <t>GPS + Cellular model</t>
   </si>
   <si>
-    <t>Digital Crown with haptic feedback; side button; Action button; Siri</t>
-  </si>
-  <si>
-    <t>Temperature sensor;7 blood oxygen sensor;4 electrical heart sensor and third-generation optical heart sensor; depth gauge; water temperature sensor</t>
-  </si>
-  <si>
-    <t>International emergency calling,10 Emergency SOS,9 Crash Detection,9 and Fall Detection; Siren</t>
-  </si>
-  <si>
-    <t>Water resistant 100 meters13</t>
-  </si>
-  <si>
     <t>Recreational dive to 40 meters</t>
   </si>
   <si>
@@ -287,18 +209,114 @@
     <t>Dual speakers and three-mic array with beamforming</t>
   </si>
   <si>
-    <t>Always-On Retina LTPO OLED display, up to 3000 nits</t>
-  </si>
-  <si>
-    <t>Digital Crown with haptic feedback; side button; Action button; double tap gesture; on-device Siri</t>
+    <t>+ depth gauge; water temperature sensor</t>
+  </si>
+  <si>
+    <t>+ Temperature sensor</t>
+  </si>
+  <si>
+    <t>+ Siren</t>
+  </si>
+  <si>
+    <t>Water resistant 100 meters</t>
+  </si>
+  <si>
+    <t>Blood oxygen sensor; electrical heart sensor and third-generation optical heart sensor</t>
+  </si>
+  <si>
+    <t>S6 SiP with 64-bit dual-core processor; W3 wireless chip; U1 chip (Ultra Wideband)</t>
+  </si>
+  <si>
+    <t>S8 SiP with 64-bit dual-core processor; W3 wireless chip; U1 chip (Ultra Wideband)</t>
+  </si>
+  <si>
+    <t>S9 SiP with 64-bit dual-core processor; W3 wireless chip; second-generation Ultra Wideband chip</t>
+  </si>
+  <si>
+    <t>+ haptic feedback</t>
+  </si>
+  <si>
+    <t>+ Siri</t>
+  </si>
+  <si>
+    <t>+ double tap gesture; on-device Siri</t>
+  </si>
+  <si>
+    <t>+ up to 3000 nits</t>
+  </si>
+  <si>
+    <t>+ up to 2000 nits</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">+ Action button; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Siri</t>
+    </r>
+  </si>
+  <si>
+    <t>+ barometric altimeter</t>
+  </si>
+  <si>
+    <t>+ compass, and always-on altimeter</t>
+  </si>
+  <si>
+    <t>+ Bluetooth 4.2</t>
+  </si>
+  <si>
+    <t>+ LTE and UMTS, and Bluetooth 5.0</t>
+  </si>
+  <si>
+    <t>+Wi-Fi 4 (802.11n), and Bluetooth 5.3</t>
+  </si>
+  <si>
+    <t>+ Fall Detection</t>
+  </si>
+  <si>
+    <t>+ International emergency calling</t>
+  </si>
+  <si>
+    <t>+ Crash Detection</t>
+  </si>
+  <si>
+    <t>+ ECG app; sleep stages</t>
+  </si>
+  <si>
+    <t>Digital Crown with haptic feedback; Action button; double tap gesture; on-device Siri</t>
+  </si>
+  <si>
+    <t>ceramic cases removed</t>
+  </si>
+  <si>
+    <t>+ sapphire crystal display on titanium and ceramic cases</t>
+  </si>
+  <si>
+    <t>- no U1 chip</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -334,15 +352,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,344 +682,370 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC167BC7-B7A1-A748-B6ED-7D5D61A18AED}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
-    <col min="6" max="6" width="20.5" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" customWidth="1"/>
-    <col min="8" max="8" width="23.5" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" customWidth="1"/>
-    <col min="10" max="10" width="24.33203125" customWidth="1"/>
-    <col min="11" max="11" width="24.6640625" customWidth="1"/>
-    <col min="12" max="12" width="27.33203125" customWidth="1"/>
-    <col min="13" max="13" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="1.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" customWidth="1"/>
+    <col min="9" max="9" width="23.5" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" customWidth="1"/>
+    <col min="11" max="11" width="24.33203125" customWidth="1"/>
+    <col min="12" max="12" width="24.6640625" customWidth="1"/>
+    <col min="13" max="13" width="27.33203125" customWidth="1"/>
+    <col min="14" max="14" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>2023</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2022</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2023</v>
+      </c>
+      <c r="E2" s="5">
+        <v>2022</v>
+      </c>
+      <c r="F2" s="5">
+        <v>2022</v>
+      </c>
+      <c r="G2" s="5">
+        <v>2021</v>
+      </c>
+      <c r="H2" s="5">
+        <v>2020</v>
+      </c>
+      <c r="I2" s="5">
+        <v>2019</v>
+      </c>
+      <c r="J2" s="5">
+        <v>2019</v>
+      </c>
+      <c r="K2" s="5">
+        <v>2018</v>
+      </c>
+      <c r="L2" s="5">
+        <v>2017</v>
+      </c>
+      <c r="M2" s="5">
+        <v>2016</v>
+      </c>
+      <c r="N2" s="5">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="2" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
+      <c r="G7" s="4"/>
+      <c r="H7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="G8" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="102" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1" t="s">
+      <c r="G9" s="1"/>
+      <c r="H9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" ht="119" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="102" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="F7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="153" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1" t="s">
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="102" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="119" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="I10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>35</v>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="N10" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="1"/>
+      <c r="B11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="6"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="6" t="s">
+        <v>78</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="J11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" s="1"/>
+      <c r="B12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="4"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1004,14 +1055,19 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="M12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="1"/>
+      <c r="B13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="4"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1022,14 +1078,15 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="B14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1039,104 +1096,125 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
-        <v>63</v>
+      <c r="E15" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="F16" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>32</v>
+      <c r="K16" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="N16" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="B17" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="L17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="B18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="4"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="I18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="1" t="s">
+      <c r="M18" s="1"/>
+      <c r="N18" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="J19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E19" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F19" t="s">
-        <v>65</v>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>